<commit_message>
Fixing taxtures for bowlstamp burned mold. Several language files. Fixed some gui sizes. Created blocks for labeled chests by wood type. Fixed files for typed chests.
</commit_message>
<xml_diff>
--- a/bin/TheNeolithicMod/Mod-spreadsheets.xlsx
+++ b/bin/TheNeolithicMod/Mod-spreadsheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\VS\Tony-Mods\The-Neolithic-Mod\bin\TheNeolithicMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD7EC0F-ED22-4133-8A96-E210E05D8DE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21811DC0-98B6-4102-BF02-B7F8D624D288}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,9 @@
     <sheet name="Darkagecraft Modpack" sheetId="3" r:id="rId3"/>
     <sheet name="Animal Spawn Rates" sheetId="4" r:id="rId4"/>
     <sheet name="Art" sheetId="5" r:id="rId5"/>
-    <sheet name="Rock Types" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1158,30 +1157,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{670E144F-73BF-468B-B618-77C827CE6BE2}" name="Table2" displayName="Table2" ref="A1:U31" totalsRowShown="0">
-  <autoFilter ref="A1:U31" xr:uid="{2901FF87-EF02-471C-8668-56E2CB2A5C08}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89D81091-1479-4F42-A671-5ABC988A208D}" name="Table2" displayName="Table2" ref="A1:U31" totalsRowShown="0">
+  <autoFilter ref="A1:U31" xr:uid="{73747813-AA2C-4C82-B659-1D22F969C982}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{70C62FDA-E67D-4785-8743-8831963150C5}" name="Rock Types and ores "/>
-    <tableColumn id="2" xr3:uid="{A399B208-2CCD-4578-9D8D-FF3CC0F4E1E1}" name="Column1"/>
-    <tableColumn id="3" xr3:uid="{A6A60EF7-7E77-4EFB-A80E-353A77D7598E}" name="Bismuthine" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{7F02E942-0CE4-4D8E-8274-5815F7D24313}" name="Cassiterite" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{F20E2C20-50C7-4F54-ADD8-65A97D9E347F}" name="Chromite" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{D1E92FAC-109A-4A87-B327-61AB9995D695}" name="Galena" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{668854B3-EA11-4B5E-9AA3-9D27F403E3B7}" name="Silver/Galena" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{45E74C23-D105-4B3C-B96E-73F32AD4D771}" name="Ilmenite" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{AA7D8378-8A87-4920-B450-7D39F7D56356}" name="Iron/Limonite" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{BAE2A965-9E10-4827-8148-B84DE8CC9EFB}" name="Iron/Hematite" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{5D812E18-D81B-47AF-84E5-29DC61A6F192}" name="Iron/Magnetite" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{BF057886-2154-470A-9844-B5FB9EAD928E}" name="Malachite" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{84CC105E-3C37-4405-852A-BAB1582E4CE9}" name="Native Copper" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{C05E682C-7D36-4A3B-8510-382B35359B4C}" name="Rhodochrosite" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{F4D2670D-E93E-4D64-9B1D-EB02C27F721A}" name="Sphalerite" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{FEDF365F-DA9F-47AA-AB6C-D03BAEE07593}" name="Quartz" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{C53971D3-7B90-487F-9233-3E5E573DC834}" name="Gold in Quartz" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{BE2A27F3-0D4C-4BB7-A266-4E685F4367C4}" name="Silver in Quartz" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{CBB02BD2-B9E9-4C91-82DB-B9F7BA520F37}" name="Column6"/>
-    <tableColumn id="20" xr3:uid="{B5259D7E-AEC8-477D-B0CB-BBF4A9F5E8D8}" name="Column7"/>
-    <tableColumn id="21" xr3:uid="{8AA3E85E-C259-4BA1-9FA7-AC17DB2ECAD1}" name="Column8"/>
+    <tableColumn id="1" xr3:uid="{A6761D79-6A6C-46B6-B5B9-CB7930F36910}" name="Rock Types and ores "/>
+    <tableColumn id="2" xr3:uid="{6EFA9C1B-0155-4298-B8EF-53CAFBFA3CEB}" name="Column1"/>
+    <tableColumn id="3" xr3:uid="{C318B405-5060-4324-8301-2F45D9CF9700}" name="Bismuthine" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1097373F-27A2-4BC5-A909-EE4A52846D2C}" name="Cassiterite" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{72C901ED-C564-460C-8EE9-1AEC4E4922C1}" name="Chromite" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{E60A8CA7-68E5-4EA0-AED0-4066969C9E27}" name="Galena" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{9CE7BA50-13CD-4A31-90C2-8CFD65F01E6F}" name="Silver/Galena" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{9A3638F0-9DFB-45A2-9E63-F63791A8134B}" name="Ilmenite" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{C0A640DC-CCB2-4F2F-9FA3-F8DFD34D2AD5}" name="Iron/Limonite" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{BE42190A-E5B0-4055-9156-EF2480FDD7C8}" name="Iron/Hematite" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{49621F09-D7F4-4B84-AB44-3B3025CC7C22}" name="Iron/Magnetite" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{8A687CB1-41E3-4279-AD2B-F501DBC30224}" name="Malachite" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{1ACAF09F-9598-4DDF-8E1D-60CB3BE3975F}" name="Native Copper" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{3A159752-C179-48AA-BE2E-E8E92AA93B7E}" name="Rhodochrosite" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{3492191C-39C0-4A1C-AA98-E43102CFDE64}" name="Sphalerite" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{102AB07F-6BF9-468E-9B8B-A039DFF76602}" name="Quartz" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{D130047F-2FFC-45D4-81D1-34523F3DF005}" name="Gold in Quartz" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{A53B182C-3050-4AD5-AB59-9FD4320BBFD0}" name="Silver in Quartz" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{F5B49C92-DD69-46A2-B46A-230A016CC472}" name="Column6"/>
+    <tableColumn id="20" xr3:uid="{D628EC43-50B7-4F11-B60B-2D4B2107DF38}" name="Column7"/>
+    <tableColumn id="21" xr3:uid="{DDC7B592-BB33-4E40-9DA7-E98BFF6BFC3D}" name="Column8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -54934,11 +54933,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374209BB-C733-44F0-9837-6C16DAD76EAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AF716A-BE6A-4F0A-BDE4-6050140BC8DF}">
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -55950,9 +55949,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>